<commit_message>
Finishing project automation xlsx file
</commit_message>
<xml_diff>
--- a/examples/project-automation/inventory.xlsx
+++ b/examples/project-automation/inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2C1EE66-BF31-4711-9E35-595E47B854B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5887C4D-392C-4443-AE1F-A4B9CD781706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="7">
   <si>
     <t>Product No</t>
   </si>
@@ -41,67 +41,13 @@
     <t>Supplier</t>
   </si>
   <si>
-    <t>200,4</t>
-  </si>
-  <si>
     <t>AAA Company</t>
   </si>
   <si>
     <t>BBB Company</t>
   </si>
   <si>
-    <t>234,99</t>
-  </si>
-  <si>
     <t>CCC Company</t>
-  </si>
-  <si>
-    <t>13,99</t>
-  </si>
-  <si>
-    <t>324,5</t>
-  </si>
-  <si>
-    <t>2352,55</t>
-  </si>
-  <si>
-    <t>9,99</t>
-  </si>
-  <si>
-    <t>19,99</t>
-  </si>
-  <si>
-    <t>200,5</t>
-  </si>
-  <si>
-    <t>234,10</t>
-  </si>
-  <si>
-    <t>14,99</t>
-  </si>
-  <si>
-    <t>324,60</t>
-  </si>
-  <si>
-    <t>2352,56</t>
-  </si>
-  <si>
-    <t>9,10</t>
-  </si>
-  <si>
-    <t>19,10</t>
-  </si>
-  <si>
-    <t>50,25</t>
-  </si>
-  <si>
-    <t>329,99</t>
-  </si>
-  <si>
-    <t>129,99</t>
-  </si>
-  <si>
-    <t>29,99</t>
   </si>
 </sst>
 </file>
@@ -459,7 +405,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,11 +437,11 @@
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="C2" s="1">
+        <v>200.4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -509,7 +455,7 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -519,11 +465,11 @@
       <c r="B4">
         <v>3000</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="1">
+        <v>234.99</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -537,7 +483,7 @@
         <v>1150</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -551,7 +497,7 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -561,11 +507,11 @@
       <c r="B7">
         <v>212</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
+      <c r="C7" s="1">
+        <v>13.99</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -575,11 +521,11 @@
       <c r="B8">
         <v>2352748</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
+      <c r="C8" s="1">
+        <v>324.5</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -589,11 +535,11 @@
       <c r="B9">
         <v>121</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
+      <c r="C9" s="1">
+        <v>2352.5500000000002</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -603,11 +549,11 @@
       <c r="B10">
         <v>212</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
+      <c r="C10" s="1">
+        <v>9.99</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -617,11 +563,11 @@
       <c r="B11">
         <v>223</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
+      <c r="C11" s="1">
+        <v>19.989999999999998</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -631,11 +577,11 @@
       <c r="B12">
         <v>745</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
+      <c r="C12" s="1">
+        <v>200.5</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -649,7 +595,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -659,11 +605,11 @@
       <c r="B14">
         <v>345</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
+      <c r="C14" s="1">
+        <v>234.1</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -677,7 +623,7 @@
         <v>1108</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -691,7 +637,7 @@
         <v>2237</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -701,11 +647,11 @@
       <c r="B17">
         <v>234</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
+      <c r="C17" s="1">
+        <v>14.99</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -715,11 +661,11 @@
       <c r="B18">
         <v>55</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
+      <c r="C18" s="1">
+        <v>324.60000000000002</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -729,11 +675,11 @@
       <c r="B19">
         <v>26</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
+      <c r="C19" s="1">
+        <v>2352.56</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -743,11 +689,11 @@
       <c r="B20">
         <v>98</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>19</v>
+      <c r="C20" s="1">
+        <v>9.1</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -757,11 +703,11 @@
       <c r="B21">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>20</v>
+      <c r="C21" s="1">
+        <v>19.100000000000001</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -771,11 +717,11 @@
       <c r="B22">
         <v>658</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>21</v>
+      <c r="C22" s="1">
+        <v>50.25</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -789,7 +735,7 @@
         <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -803,7 +749,7 @@
         <v>199</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -817,7 +763,7 @@
         <v>299</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -827,11 +773,11 @@
       <c r="B26">
         <v>233</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>22</v>
+      <c r="C26" s="1">
+        <v>329.99</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -841,11 +787,11 @@
       <c r="B27">
         <v>244</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>23</v>
+      <c r="C27" s="1">
+        <v>129.99</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -855,11 +801,11 @@
       <c r="B28">
         <v>100</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
+      <c r="C28" s="1">
+        <v>29.99</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -873,7 +819,7 @@
         <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -887,7 +833,7 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>